<commit_message>
adjust wordings in rmd file and create html output
</commit_message>
<xml_diff>
--- a/MDS_graph.xlsx
+++ b/MDS_graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allenyang/Box/GDM_assessment/GDM_assessment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3A99CE-8E1E-8F45-94B2-06ED941294EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24D55F7-4BA0-9F4E-AD09-4D7500AF623A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart2" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="9">
   <si>
     <t>Days after 5/1</t>
   </si>
@@ -572,7 +572,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -580,6 +580,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -801,76 +802,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>32.789583333333326</c:v>
+                  <c:v>-5.8604166666666657</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.8104166666666828</c:v>
+                  <c:v>5.0895833333333371</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.1895833333333172</c:v>
+                  <c:v>13.28958333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7895833333333258</c:v>
+                  <c:v>-6.4104166666666629</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0895833333333229</c:v>
+                  <c:v>4.0895833333333371</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.38958333333332</c:v>
+                  <c:v>32.78958333333334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5.2104166666666742</c:v>
+                  <c:v>-3.8104166666666686</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5895833333333229</c:v>
+                  <c:v>8.1895833333333314</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.38958333333332007</c:v>
+                  <c:v>6.78958333333334</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-19.010416666666679</c:v>
+                  <c:v>16.389583333333334</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-6.4104166666666771</c:v>
+                  <c:v>-5.21041666666666</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.1895833333333172</c:v>
+                  <c:v>2.5895833333333371</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-14.210416666666681</c:v>
+                  <c:v>0.38958333333333428</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.58958333333332291</c:v>
+                  <c:v>-19.010416666666664</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.989583333333314</c:v>
+                  <c:v>4.1895833333333314</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-1.1104166666666799</c:v>
+                  <c:v>-14.210416666666667</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.2104166666666742</c:v>
+                  <c:v>0.58958333333333712</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-8.2104166666666814</c:v>
+                  <c:v>14.989583333333329</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-4.9104166666666771</c:v>
+                  <c:v>-1.1104166666666657</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-12.810416666666683</c:v>
+                  <c:v>-2.21041666666666</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-25.61041666666668</c:v>
+                  <c:v>-8.2104166666666671</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13.289583333333326</c:v>
+                  <c:v>-4.9104166666666629</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.0895833333333229</c:v>
+                  <c:v>-12.810416666666669</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-5.8604166666666799</c:v>
+                  <c:v>-25.610416666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -993,76 +994,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>27.634583333333339</c:v>
+                  <c:v>-3.4954166666666566</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.1654166666666583</c:v>
+                  <c:v>7.1345833333333388</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7345833333333331</c:v>
+                  <c:v>11.334583333333342</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.434583333333336</c:v>
+                  <c:v>18.034583333333345</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>8.3345833333333417</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>27.634583333333339</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.1654166666666583</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7345833333333331</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.434583333333336</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>19.434583333333336</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>-8.6654166666666583</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.8345833333333417</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1.1654166666666583</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-22.465416666666663</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>18.034583333333345</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2.8345833333333417</c:v>
                 </c:pt>
                 <c:pt idx="12">
+                  <c:v>-1.1654166666666583</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-22.465416666666663</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.8345833333333417</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>-16.365416666666661</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>-2.065416666666664</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>15.434583333333336</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>-1.565416666666664</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>-4.065416666666664</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>-10.26541666666666</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>-5.4654166666666555</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>-8.8654166666666612</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>-31.565416666666664</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>11.334583333333342</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.1345833333333388</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-3.4954166666666566</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1185,76 +1186,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>31.279166666666669</c:v>
+                  <c:v>-6.7208333333333456</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7.1208333333333229</c:v>
+                  <c:v>7.4791666666666572</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9791666666666714</c:v>
+                  <c:v>13.979166666666657</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.7791666666666686</c:v>
+                  <c:v>4.17916666666666</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3791666666666771</c:v>
+                  <c:v>8.3791666666666629</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.479166666666671</c:v>
+                  <c:v>31.279166666666654</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9.9208333333333201</c:v>
+                  <c:v>-7.1208333333333371</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.8208333333333258</c:v>
+                  <c:v>5.9791666666666572</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.9791666666666714</c:v>
+                  <c:v>8.7791666666666544</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-21.320833333333326</c:v>
+                  <c:v>16.479166666666657</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.1791666666666742</c:v>
+                  <c:v>-9.9208333333333343</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.3791666666666771</c:v>
+                  <c:v>-1.82083333333334</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-15.320833333333326</c:v>
+                  <c:v>2.9791666666666572</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3791666666666771</c:v>
+                  <c:v>-21.32083333333334</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.179166666666674</c:v>
+                  <c:v>4.3791666666666629</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.1208333333333229</c:v>
+                  <c:v>-15.32083333333334</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.7208333333333314</c:v>
+                  <c:v>2.3791666666666629</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-10.320833333333326</c:v>
+                  <c:v>15.17916666666666</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0791666666666799</c:v>
+                  <c:v>-2.1208333333333371</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-13.620833333333323</c:v>
+                  <c:v>-2.7208333333333456</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-32.520833333333329</c:v>
+                  <c:v>-10.32083333333334</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13.979166666666671</c:v>
+                  <c:v>2.0791666666666657</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.4791666666666714</c:v>
+                  <c:v>-13.620833333333337</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-6.7208333333333314</c:v>
+                  <c:v>-32.520833333333343</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1377,76 +1378,76 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>31.512499999999989</c:v>
+                  <c:v>-3.9875000000000114</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.1875000000000142</c:v>
+                  <c:v>7.3124999999999858</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6124999999999829</c:v>
+                  <c:v>13.912499999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0124999999999886</c:v>
+                  <c:v>-10.387500000000017</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>9.4124999999999943</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>31.512499999999989</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5.1875000000000142</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.6124999999999829</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0124999999999886</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>19.412499999999994</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="10">
                   <c:v>-9.1875000000000142</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="11">
                   <c:v>0.11249999999998295</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="12">
                   <c:v>3.3124999999999858</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="13">
                   <c:v>-19.987500000000011</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>-10.387500000000017</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>3.1124999999999829</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="15">
                   <c:v>-15.487500000000011</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="16">
                   <c:v>2.7124999999999915</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="17">
                   <c:v>17.212499999999991</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>2.2124999999999915</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="19">
                   <c:v>-0.58750000000000568</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="20">
                   <c:v>-8.2875000000000085</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="21">
                   <c:v>-8.7500000000005684E-2</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="22">
                   <c:v>-14.987500000000011</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="23">
                   <c:v>-34.687500000000014</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>13.912499999999994</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.3124999999999858</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-3.9875000000000114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3747,7 +3748,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="140" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3769,7 +3770,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9298214" cy="6059714"/>
+    <xdr:ext cx="9306560" cy="6075680"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -4130,7 +4131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D05B39A-54B8-F448-843E-DDED3BF98CA2}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
@@ -4194,7 +4195,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B25"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4234,7 +4235,7 @@
         <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M1" t="s">
         <v>1</v>
@@ -4288,20 +4289,24 @@
         <f t="shared" si="0"/>
         <v>2.8199999999999932</v>
       </c>
-      <c r="L2" s="1">
-        <v>43587</v>
+      <c r="L2">
+        <v>-14</v>
       </c>
       <c r="M2">
-        <v>32.789583333333326</v>
+        <f>C2-$C$27</f>
+        <v>-5.8604166666666657</v>
       </c>
       <c r="N2">
-        <v>27.634583333333339</v>
+        <f>D2-$D$27</f>
+        <v>-3.4954166666666566</v>
       </c>
       <c r="O2">
-        <v>31.279166666666669</v>
+        <f>E2-$E$27</f>
+        <v>-6.7208333333333456</v>
       </c>
       <c r="P2">
-        <v>31.512499999999989</v>
+        <f>F2-$F$27</f>
+        <v>-3.9875000000000114</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -4344,25 +4349,29 @@
         <f t="shared" ref="K3:K25" si="5">F3-$G3</f>
         <v>2.3499999999999943</v>
       </c>
-      <c r="L3" s="1">
-        <v>43591</v>
+      <c r="L3">
+        <v>-8</v>
       </c>
       <c r="M3">
-        <v>-3.8104166666666828</v>
+        <f t="shared" ref="M3:M25" si="6">C3-$C$27</f>
+        <v>5.0895833333333371</v>
       </c>
       <c r="N3">
-        <v>-5.1654166666666583</v>
+        <f t="shared" ref="N3:N25" si="7">D3-$D$27</f>
+        <v>7.1345833333333388</v>
       </c>
       <c r="O3">
-        <v>-7.1208333333333229</v>
+        <f t="shared" ref="O3:O25" si="8">E3-$E$27</f>
+        <v>7.4791666666666572</v>
       </c>
       <c r="P3">
-        <v>-5.1875000000000142</v>
+        <f t="shared" ref="P3:P25" si="9">F3-$F$27</f>
+        <v>7.3124999999999858</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1">
-        <f t="shared" ref="A4:A25" si="6">$A$2+$B4-1</f>
+        <f t="shared" ref="A4:A25" si="10">$A$2+$B4-1</f>
         <v>43580</v>
       </c>
       <c r="B4">
@@ -4400,25 +4409,29 @@
         <f t="shared" si="5"/>
         <v>2.5749999999999886</v>
       </c>
-      <c r="L4" s="1">
-        <v>43593</v>
+      <c r="L4">
+        <v>-6</v>
       </c>
       <c r="M4">
-        <v>8.1895833333333172</v>
+        <f t="shared" si="6"/>
+        <v>13.28958333333334</v>
       </c>
       <c r="N4">
-        <v>2.7345833333333331</v>
+        <f t="shared" si="7"/>
+        <v>11.334583333333342</v>
       </c>
       <c r="O4">
-        <v>5.9791666666666714</v>
+        <f t="shared" si="8"/>
+        <v>13.979166666666657</v>
       </c>
       <c r="P4">
-        <v>4.6124999999999829</v>
+        <f t="shared" si="9"/>
+        <v>13.912499999999994</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43584</v>
       </c>
       <c r="B5">
@@ -4456,25 +4469,29 @@
         <f t="shared" si="5"/>
         <v>-9.9500000000000171</v>
       </c>
-      <c r="L5" s="1">
-        <v>43595</v>
+      <c r="L5">
+        <v>-2</v>
       </c>
       <c r="M5">
-        <v>6.7895833333333258</v>
+        <f t="shared" si="6"/>
+        <v>-6.4104166666666629</v>
       </c>
       <c r="N5">
-        <v>5.434583333333336</v>
+        <f t="shared" si="7"/>
+        <v>18.034583333333345</v>
       </c>
       <c r="O5">
-        <v>8.7791666666666686</v>
+        <f t="shared" si="8"/>
+        <v>4.17916666666666</v>
       </c>
       <c r="P5">
-        <v>8.0124999999999886</v>
+        <f t="shared" si="9"/>
+        <v>-10.387500000000017</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43585</v>
       </c>
       <c r="B6">
@@ -4512,25 +4529,29 @@
         <f t="shared" si="5"/>
         <v>3.6500000000000057</v>
       </c>
-      <c r="L6" s="1">
-        <v>43585</v>
+      <c r="L6">
+        <v>-1</v>
       </c>
       <c r="M6">
-        <v>4.0895833333333229</v>
+        <f t="shared" si="6"/>
+        <v>4.0895833333333371</v>
       </c>
       <c r="N6">
+        <f t="shared" si="7"/>
         <v>8.3345833333333417</v>
       </c>
       <c r="O6">
-        <v>8.3791666666666771</v>
+        <f t="shared" si="8"/>
+        <v>8.3791666666666629</v>
       </c>
       <c r="P6">
+        <f t="shared" si="9"/>
         <v>9.4124999999999943</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43587</v>
       </c>
       <c r="B7">
@@ -4568,25 +4589,29 @@
         <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
-      <c r="L7" s="1">
-        <v>43600</v>
+      <c r="L7">
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>16.38958333333332</v>
+        <f t="shared" si="6"/>
+        <v>32.78958333333334</v>
       </c>
       <c r="N7">
-        <v>19.434583333333336</v>
+        <f t="shared" si="7"/>
+        <v>27.634583333333339</v>
       </c>
       <c r="O7">
-        <v>16.479166666666671</v>
+        <f t="shared" si="8"/>
+        <v>31.279166666666654</v>
       </c>
       <c r="P7">
-        <v>19.412499999999994</v>
+        <f t="shared" si="9"/>
+        <v>31.512499999999989</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43591</v>
       </c>
       <c r="B8">
@@ -4624,25 +4649,29 @@
         <f t="shared" si="5"/>
         <v>1.9249999999999972</v>
       </c>
-      <c r="L8" s="1">
-        <v>43601</v>
+      <c r="L8">
+        <v>5</v>
       </c>
       <c r="M8">
-        <v>-5.2104166666666742</v>
+        <f t="shared" si="6"/>
+        <v>-3.8104166666666686</v>
       </c>
       <c r="N8">
-        <v>-8.6654166666666583</v>
+        <f t="shared" si="7"/>
+        <v>-5.1654166666666583</v>
       </c>
       <c r="O8">
-        <v>-9.9208333333333201</v>
+        <f t="shared" si="8"/>
+        <v>-7.1208333333333371</v>
       </c>
       <c r="P8">
-        <v>-9.1875000000000142</v>
+        <f t="shared" si="9"/>
+        <v>-5.1875000000000142</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43593</v>
       </c>
       <c r="B9">
@@ -4680,25 +4709,29 @@
         <f t="shared" si="5"/>
         <v>1.0250000000000057</v>
       </c>
-      <c r="L9" s="1">
-        <v>43602</v>
+      <c r="L9">
+        <v>7</v>
       </c>
       <c r="M9">
-        <v>2.5895833333333229</v>
+        <f t="shared" si="6"/>
+        <v>8.1895833333333314</v>
       </c>
       <c r="N9">
-        <v>2.8345833333333417</v>
+        <f t="shared" si="7"/>
+        <v>2.7345833333333331</v>
       </c>
       <c r="O9">
-        <v>-1.8208333333333258</v>
+        <f t="shared" si="8"/>
+        <v>5.9791666666666572</v>
       </c>
       <c r="P9">
-        <v>0.11249999999998295</v>
+        <f t="shared" si="9"/>
+        <v>4.6124999999999829</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43595</v>
       </c>
       <c r="B10">
@@ -4736,25 +4769,29 @@
         <f t="shared" si="5"/>
         <v>2.5500000000000114</v>
       </c>
-      <c r="L10" s="1">
-        <v>43603</v>
+      <c r="L10">
+        <v>9</v>
       </c>
       <c r="M10">
-        <v>0.38958333333332007</v>
+        <f t="shared" si="6"/>
+        <v>6.78958333333334</v>
       </c>
       <c r="N10">
-        <v>-1.1654166666666583</v>
+        <f t="shared" si="7"/>
+        <v>5.434583333333336</v>
       </c>
       <c r="O10">
-        <v>2.9791666666666714</v>
+        <f t="shared" si="8"/>
+        <v>8.7791666666666544</v>
       </c>
       <c r="P10">
-        <v>3.3124999999999858</v>
+        <f t="shared" si="9"/>
+        <v>8.0124999999999886</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43600</v>
       </c>
       <c r="B11">
@@ -4792,25 +4829,29 @@
         <f t="shared" si="5"/>
         <v>3.2750000000000057</v>
       </c>
-      <c r="L11" s="1">
-        <v>43605</v>
+      <c r="L11">
+        <v>14</v>
       </c>
       <c r="M11">
-        <v>-19.010416666666679</v>
+        <f t="shared" si="6"/>
+        <v>16.389583333333334</v>
       </c>
       <c r="N11">
-        <v>-22.465416666666663</v>
+        <f t="shared" si="7"/>
+        <v>19.434583333333336</v>
       </c>
       <c r="O11">
-        <v>-21.320833333333326</v>
+        <f t="shared" si="8"/>
+        <v>16.479166666666657</v>
       </c>
       <c r="P11">
-        <v>-19.987500000000011</v>
+        <f t="shared" si="9"/>
+        <v>19.412499999999994</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43601</v>
       </c>
       <c r="B12">
@@ -4848,25 +4889,29 @@
         <f t="shared" si="5"/>
         <v>0.84999999999999432</v>
       </c>
-      <c r="L12" s="1">
-        <v>43584</v>
+      <c r="L12">
+        <v>15</v>
       </c>
       <c r="M12">
-        <v>-6.4104166666666771</v>
+        <f t="shared" si="6"/>
+        <v>-5.21041666666666</v>
       </c>
       <c r="N12">
-        <v>18.034583333333345</v>
+        <f t="shared" si="7"/>
+        <v>-8.6654166666666583</v>
       </c>
       <c r="O12">
-        <v>4.1791666666666742</v>
+        <f t="shared" si="8"/>
+        <v>-9.9208333333333343</v>
       </c>
       <c r="P12">
-        <v>-10.387500000000017</v>
+        <f t="shared" si="9"/>
+        <v>-9.1875000000000142</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43602</v>
       </c>
       <c r="B13">
@@ -4904,25 +4949,29 @@
         <f t="shared" si="5"/>
         <v>0.97499999999999432</v>
       </c>
-      <c r="L13" s="1">
-        <v>43606</v>
+      <c r="L13">
+        <v>16</v>
       </c>
       <c r="M13">
-        <v>4.1895833333333172</v>
+        <f t="shared" si="6"/>
+        <v>2.5895833333333371</v>
       </c>
       <c r="N13">
+        <f t="shared" si="7"/>
         <v>2.8345833333333417</v>
       </c>
       <c r="O13">
-        <v>4.3791666666666771</v>
+        <f t="shared" si="8"/>
+        <v>-1.82083333333334</v>
       </c>
       <c r="P13">
-        <v>3.1124999999999829</v>
+        <f t="shared" si="9"/>
+        <v>0.11249999999998295</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43603</v>
       </c>
       <c r="B14">
@@ -4960,25 +5009,29 @@
         <f t="shared" si="5"/>
         <v>3.7249999999999943</v>
       </c>
-      <c r="L14" s="1">
-        <v>43607</v>
+      <c r="L14">
+        <v>17</v>
       </c>
       <c r="M14">
-        <v>-14.210416666666681</v>
+        <f t="shared" si="6"/>
+        <v>0.38958333333333428</v>
       </c>
       <c r="N14">
-        <v>-16.365416666666661</v>
+        <f t="shared" si="7"/>
+        <v>-1.1654166666666583</v>
       </c>
       <c r="O14">
-        <v>-15.320833333333326</v>
+        <f t="shared" si="8"/>
+        <v>2.9791666666666572</v>
       </c>
       <c r="P14">
-        <v>-15.487500000000011</v>
+        <f t="shared" si="9"/>
+        <v>3.3124999999999858</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43605</v>
       </c>
       <c r="B15">
@@ -5016,25 +5069,29 @@
         <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
-      <c r="L15" s="1">
-        <v>43608</v>
+      <c r="L15">
+        <v>19</v>
       </c>
       <c r="M15">
-        <v>0.58958333333332291</v>
+        <f t="shared" si="6"/>
+        <v>-19.010416666666664</v>
       </c>
       <c r="N15">
-        <v>-2.065416666666664</v>
+        <f t="shared" si="7"/>
+        <v>-22.465416666666663</v>
       </c>
       <c r="O15">
-        <v>2.3791666666666771</v>
+        <f t="shared" si="8"/>
+        <v>-21.32083333333334</v>
       </c>
       <c r="P15">
-        <v>2.7124999999999915</v>
+        <f t="shared" si="9"/>
+        <v>-19.987500000000011</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43606</v>
       </c>
       <c r="B16">
@@ -5072,25 +5129,29 @@
         <f t="shared" si="5"/>
         <v>1.2750000000000057</v>
       </c>
-      <c r="L16" s="1">
-        <v>43609</v>
+      <c r="L16">
+        <v>20</v>
       </c>
       <c r="M16">
-        <v>14.989583333333314</v>
+        <f t="shared" si="6"/>
+        <v>4.1895833333333314</v>
       </c>
       <c r="N16">
-        <v>15.434583333333336</v>
+        <f t="shared" si="7"/>
+        <v>2.8345833333333417</v>
       </c>
       <c r="O16">
-        <v>15.179166666666674</v>
+        <f t="shared" si="8"/>
+        <v>4.3791666666666629</v>
       </c>
       <c r="P16">
-        <v>17.212499999999991</v>
+        <f t="shared" si="9"/>
+        <v>3.1124999999999829</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43607</v>
       </c>
       <c r="B17">
@@ -5128,25 +5189,29 @@
         <f t="shared" si="5"/>
         <v>1.6499999999999986</v>
       </c>
-      <c r="L17" s="1">
-        <v>43610</v>
+      <c r="L17">
+        <v>21</v>
       </c>
       <c r="M17">
-        <v>-1.1104166666666799</v>
+        <f t="shared" si="6"/>
+        <v>-14.210416666666667</v>
       </c>
       <c r="N17">
-        <v>-1.565416666666664</v>
+        <f t="shared" si="7"/>
+        <v>-16.365416666666661</v>
       </c>
       <c r="O17">
-        <v>-2.1208333333333229</v>
+        <f t="shared" si="8"/>
+        <v>-15.32083333333334</v>
       </c>
       <c r="P17">
-        <v>2.2124999999999915</v>
+        <f t="shared" si="9"/>
+        <v>-15.487500000000011</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43608</v>
       </c>
       <c r="B18">
@@ -5184,25 +5249,29 @@
         <f t="shared" si="5"/>
         <v>3.6000000000000085</v>
       </c>
-      <c r="L18" s="1">
-        <v>43611</v>
+      <c r="L18">
+        <v>22</v>
       </c>
       <c r="M18">
-        <v>-2.2104166666666742</v>
+        <f t="shared" si="6"/>
+        <v>0.58958333333333712</v>
       </c>
       <c r="N18">
-        <v>-4.065416666666664</v>
+        <f t="shared" si="7"/>
+        <v>-2.065416666666664</v>
       </c>
       <c r="O18">
-        <v>-2.7208333333333314</v>
+        <f t="shared" si="8"/>
+        <v>2.3791666666666629</v>
       </c>
       <c r="P18">
-        <v>-0.58750000000000568</v>
+        <f t="shared" si="9"/>
+        <v>2.7124999999999915</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43609</v>
       </c>
       <c r="B19">
@@ -5240,25 +5309,29 @@
         <f t="shared" si="5"/>
         <v>3.3000000000000114</v>
       </c>
-      <c r="L19" s="1">
-        <v>43612</v>
+      <c r="L19">
+        <v>23</v>
       </c>
       <c r="M19">
-        <v>-8.2104166666666814</v>
+        <f t="shared" si="6"/>
+        <v>14.989583333333329</v>
       </c>
       <c r="N19">
-        <v>-10.26541666666666</v>
+        <f t="shared" si="7"/>
+        <v>15.434583333333336</v>
       </c>
       <c r="O19">
-        <v>-10.320833333333326</v>
+        <f t="shared" si="8"/>
+        <v>15.17916666666666</v>
       </c>
       <c r="P19">
-        <v>-8.2875000000000085</v>
+        <f t="shared" si="9"/>
+        <v>17.212499999999991</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43610</v>
       </c>
       <c r="B20">
@@ -5296,25 +5369,29 @@
         <f t="shared" si="5"/>
         <v>4.6500000000000057</v>
       </c>
-      <c r="L20" s="1">
-        <v>43613</v>
+      <c r="L20">
+        <v>24</v>
       </c>
       <c r="M20">
-        <v>-4.9104166666666771</v>
+        <f t="shared" si="6"/>
+        <v>-1.1104166666666657</v>
       </c>
       <c r="N20">
-        <v>-5.4654166666666555</v>
+        <f t="shared" si="7"/>
+        <v>-1.565416666666664</v>
       </c>
       <c r="O20">
-        <v>2.0791666666666799</v>
+        <f t="shared" si="8"/>
+        <v>-2.1208333333333371</v>
       </c>
       <c r="P20">
-        <v>-8.7500000000005684E-2</v>
+        <f t="shared" si="9"/>
+        <v>2.2124999999999915</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43611</v>
       </c>
       <c r="B21">
@@ -5352,25 +5429,29 @@
         <f t="shared" si="5"/>
         <v>3.6000000000000085</v>
       </c>
-      <c r="L21" s="1">
-        <v>43616</v>
+      <c r="L21">
+        <v>25</v>
       </c>
       <c r="M21">
-        <v>-12.810416666666683</v>
+        <f t="shared" si="6"/>
+        <v>-2.21041666666666</v>
       </c>
       <c r="N21">
-        <v>-8.8654166666666612</v>
+        <f t="shared" si="7"/>
+        <v>-4.065416666666664</v>
       </c>
       <c r="O21">
-        <v>-13.620833333333323</v>
+        <f t="shared" si="8"/>
+        <v>-2.7208333333333456</v>
       </c>
       <c r="P21">
-        <v>-14.987500000000011</v>
+        <f t="shared" si="9"/>
+        <v>-0.58750000000000568</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43612</v>
       </c>
       <c r="B22">
@@ -5408,25 +5489,29 @@
         <f t="shared" si="5"/>
         <v>2.7750000000000057</v>
       </c>
-      <c r="L22" s="1">
-        <v>43629</v>
+      <c r="L22">
+        <v>26</v>
       </c>
       <c r="M22">
-        <v>-25.61041666666668</v>
+        <f t="shared" si="6"/>
+        <v>-8.2104166666666671</v>
       </c>
       <c r="N22">
-        <v>-31.565416666666664</v>
+        <f t="shared" si="7"/>
+        <v>-10.26541666666666</v>
       </c>
       <c r="O22">
-        <v>-32.520833333333329</v>
+        <f t="shared" si="8"/>
+        <v>-10.32083333333334</v>
       </c>
       <c r="P22">
-        <v>-34.687500000000014</v>
+        <f t="shared" si="9"/>
+        <v>-8.2875000000000085</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43613</v>
       </c>
       <c r="B23">
@@ -5464,25 +5549,29 @@
         <f t="shared" si="5"/>
         <v>3.7999999999999972</v>
       </c>
-      <c r="L23" s="1">
-        <v>43580</v>
+      <c r="L23">
+        <v>27</v>
       </c>
       <c r="M23">
-        <v>13.289583333333326</v>
+        <f t="shared" si="6"/>
+        <v>-4.9104166666666629</v>
       </c>
       <c r="N23">
-        <v>11.334583333333342</v>
+        <f t="shared" si="7"/>
+        <v>-5.4654166666666555</v>
       </c>
       <c r="O23">
-        <v>13.979166666666671</v>
+        <f t="shared" si="8"/>
+        <v>2.0791666666666657</v>
       </c>
       <c r="P23">
-        <v>13.912499999999994</v>
+        <f t="shared" si="9"/>
+        <v>-8.7500000000005684E-2</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43616</v>
       </c>
       <c r="B24">
@@ -5520,25 +5609,29 @@
         <f t="shared" si="5"/>
         <v>-0.625</v>
       </c>
-      <c r="L24" s="1">
-        <v>43578</v>
+      <c r="L24">
+        <v>30</v>
       </c>
       <c r="M24">
-        <v>5.0895833333333229</v>
+        <f t="shared" si="6"/>
+        <v>-12.810416666666669</v>
       </c>
       <c r="N24">
-        <v>7.1345833333333388</v>
+        <f t="shared" si="7"/>
+        <v>-8.8654166666666612</v>
       </c>
       <c r="O24">
-        <v>7.4791666666666714</v>
+        <f t="shared" si="8"/>
+        <v>-13.620833333333337</v>
       </c>
       <c r="P24">
-        <v>7.3124999999999858</v>
+        <f t="shared" si="9"/>
+        <v>-14.987500000000011</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>43629</v>
       </c>
       <c r="B25">
@@ -5576,20 +5669,24 @@
         <f t="shared" si="5"/>
         <v>-1.7999999999999972</v>
       </c>
-      <c r="L25" s="1">
-        <v>43572</v>
+      <c r="L25">
+        <v>43</v>
       </c>
       <c r="M25">
-        <v>-5.8604166666666799</v>
+        <f t="shared" si="6"/>
+        <v>-25.610416666666666</v>
       </c>
       <c r="N25">
-        <v>-3.4954166666666566</v>
+        <f t="shared" si="7"/>
+        <v>-31.565416666666664</v>
       </c>
       <c r="O25">
-        <v>-6.7208333333333314</v>
+        <f t="shared" si="8"/>
+        <v>-32.520833333333343</v>
       </c>
       <c r="P25">
-        <v>-3.9875000000000114</v>
+        <f t="shared" si="9"/>
+        <v>-34.687500000000014</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -5598,15 +5695,15 @@
         <v>70.110416666666666</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:F27" si="7">AVERAGE(D2:D25)</f>
+        <f t="shared" ref="D27:F27" si="11">AVERAGE(D2:D25)</f>
         <v>73.365416666666661</v>
       </c>
       <c r="E27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>77.32083333333334</v>
       </c>
       <c r="F27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>75.987500000000011</v>
       </c>
     </row>
@@ -5626,8 +5723,1587 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:P25">
-    <cfRule type="colorScale" priority="1">
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AR25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3:AR7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="35" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="40" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="44" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:44">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44">
+      <c r="A2" s="1">
+        <v>43629</v>
+      </c>
+      <c r="B2">
+        <v>-25.61041666666668</v>
+      </c>
+      <c r="C2">
+        <v>-31.565416666666664</v>
+      </c>
+      <c r="D2">
+        <v>-32.520833333333329</v>
+      </c>
+      <c r="E2">
+        <v>-34.687500000000014</v>
+      </c>
+      <c r="G2" s="1">
+        <v>43587</v>
+      </c>
+      <c r="H2">
+        <v>-2.0999999999999943</v>
+      </c>
+      <c r="I2">
+        <v>-4</v>
+      </c>
+      <c r="J2">
+        <v>2.5</v>
+      </c>
+      <c r="K2">
+        <v>3.5999999999999943</v>
+      </c>
+      <c r="M2">
+        <v>43</v>
+      </c>
+      <c r="N2">
+        <v>-25.610416666666701</v>
+      </c>
+      <c r="O2">
+        <v>-31.565416666666664</v>
+      </c>
+      <c r="P2">
+        <v>-32.520833333333343</v>
+      </c>
+      <c r="Q2">
+        <v>-34.687500000000014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44">
+      <c r="A3" s="1">
+        <v>43605</v>
+      </c>
+      <c r="B3">
+        <v>-19.010416666666679</v>
+      </c>
+      <c r="C3">
+        <v>-22.465416666666663</v>
+      </c>
+      <c r="D3">
+        <v>-21.320833333333326</v>
+      </c>
+      <c r="E3">
+        <v>-19.987500000000011</v>
+      </c>
+      <c r="G3" s="1">
+        <v>43591</v>
+      </c>
+      <c r="H3">
+        <v>-2.5750000000000028</v>
+      </c>
+      <c r="I3">
+        <v>-0.67499999999999716</v>
+      </c>
+      <c r="J3">
+        <v>1.9249999999999972</v>
+      </c>
+      <c r="K3">
+        <v>1.3250000000000028</v>
+      </c>
+      <c r="M3">
+        <v>19</v>
+      </c>
+      <c r="N3">
+        <v>-19.010416666666664</v>
+      </c>
+      <c r="O3">
+        <v>-22.465416666666663</v>
+      </c>
+      <c r="P3">
+        <v>-21.32083333333334</v>
+      </c>
+      <c r="Q3">
+        <v>-19.987500000000011</v>
+      </c>
+      <c r="T3" t="s">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>43</v>
+      </c>
+      <c r="V3">
+        <v>19</v>
+      </c>
+      <c r="W3">
+        <v>21</v>
+      </c>
+      <c r="X3">
+        <v>30</v>
+      </c>
+      <c r="Y3">
+        <v>26</v>
+      </c>
+      <c r="Z3">
+        <v>-2</v>
+      </c>
+      <c r="AA3">
+        <v>-14</v>
+      </c>
+      <c r="AB3">
+        <v>15</v>
+      </c>
+      <c r="AC3">
+        <v>27</v>
+      </c>
+      <c r="AD3">
+        <v>5</v>
+      </c>
+      <c r="AE3">
+        <v>25</v>
+      </c>
+      <c r="AF3">
+        <v>24</v>
+      </c>
+      <c r="AG3">
+        <v>17</v>
+      </c>
+      <c r="AH3">
+        <v>22</v>
+      </c>
+      <c r="AI3">
+        <v>16</v>
+      </c>
+      <c r="AJ3">
+        <v>-1</v>
+      </c>
+      <c r="AK3">
+        <v>20</v>
+      </c>
+      <c r="AL3">
+        <v>-8</v>
+      </c>
+      <c r="AM3">
+        <v>9</v>
+      </c>
+      <c r="AN3">
+        <v>7</v>
+      </c>
+      <c r="AO3">
+        <v>-6</v>
+      </c>
+      <c r="AP3">
+        <v>23</v>
+      </c>
+      <c r="AQ3">
+        <v>14</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44">
+      <c r="A4" s="1">
+        <v>43607</v>
+      </c>
+      <c r="B4">
+        <v>-14.210416666666681</v>
+      </c>
+      <c r="C4">
+        <v>-16.365416666666661</v>
+      </c>
+      <c r="D4">
+        <v>-15.320833333333326</v>
+      </c>
+      <c r="E4">
+        <v>-15.487500000000011</v>
+      </c>
+      <c r="G4" s="1">
+        <v>43593</v>
+      </c>
+      <c r="H4">
+        <v>-1.2749999999999915</v>
+      </c>
+      <c r="I4">
+        <v>-3.4749999999999943</v>
+      </c>
+      <c r="J4">
+        <v>1.0250000000000057</v>
+      </c>
+      <c r="K4">
+        <v>3.7250000000000085</v>
+      </c>
+      <c r="M4">
+        <v>21</v>
+      </c>
+      <c r="N4">
+        <v>-14.210416666666667</v>
+      </c>
+      <c r="O4">
+        <v>-16.365416666666661</v>
+      </c>
+      <c r="P4">
+        <v>-15.32083333333334</v>
+      </c>
+      <c r="Q4">
+        <v>-15.487500000000011</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" s="5">
+        <v>-25.610416666666701</v>
+      </c>
+      <c r="V4" s="5">
+        <v>-19.010416666666664</v>
+      </c>
+      <c r="W4" s="5">
+        <v>-14.210416666666667</v>
+      </c>
+      <c r="X4" s="5">
+        <v>-12.810416666666669</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>-8.2104166666666671</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>-6.4104166666666629</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>-5.8604166666666657</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>-5.21041666666666</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>-4.9104166666666629</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>-3.8104166666666686</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>-2.21041666666666</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>-1.1104166666666657</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>0.38958333333333428</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0.58958333333333712</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>2.5895833333333371</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>4.0895833333333371</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>4.1895833333333314</v>
+      </c>
+      <c r="AL4" s="5">
+        <v>5.0895833333333371</v>
+      </c>
+      <c r="AM4" s="5">
+        <v>6.78958333333334</v>
+      </c>
+      <c r="AN4" s="5">
+        <v>8.1895833333333314</v>
+      </c>
+      <c r="AO4" s="5">
+        <v>13.28958333333334</v>
+      </c>
+      <c r="AP4" s="5">
+        <v>14.989583333333329</v>
+      </c>
+      <c r="AQ4" s="5">
+        <v>16.389583333333334</v>
+      </c>
+      <c r="AR4" s="5">
+        <v>32.78958333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44">
+      <c r="A5" s="1">
+        <v>43616</v>
+      </c>
+      <c r="B5">
+        <v>-12.810416666666683</v>
+      </c>
+      <c r="C5">
+        <v>-8.8654166666666612</v>
+      </c>
+      <c r="D5">
+        <v>-13.620833333333323</v>
+      </c>
+      <c r="E5">
+        <v>-14.987500000000011</v>
+      </c>
+      <c r="G5" s="1">
+        <v>43595</v>
+      </c>
+      <c r="H5">
+        <v>-4.5499999999999829</v>
+      </c>
+      <c r="I5">
+        <v>-2.6499999999999915</v>
+      </c>
+      <c r="J5">
+        <v>2.5500000000000114</v>
+      </c>
+      <c r="K5">
+        <v>4.6500000000000057</v>
+      </c>
+      <c r="M5">
+        <v>30</v>
+      </c>
+      <c r="N5">
+        <v>-12.810416666666669</v>
+      </c>
+      <c r="O5">
+        <v>-8.8654166666666612</v>
+      </c>
+      <c r="P5">
+        <v>-13.620833333333337</v>
+      </c>
+      <c r="Q5">
+        <v>-14.987500000000011</v>
+      </c>
+      <c r="T5" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="5">
+        <v>-31.565416666666664</v>
+      </c>
+      <c r="V5" s="5">
+        <v>-22.465416666666663</v>
+      </c>
+      <c r="W5" s="5">
+        <v>-16.365416666666661</v>
+      </c>
+      <c r="X5" s="5">
+        <v>-8.8654166666666612</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>-10.26541666666666</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>18.034583333333345</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>-3.4954166666666566</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>-8.6654166666666583</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>-5.4654166666666555</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>-5.1654166666666583</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>-4.065416666666664</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>-1.565416666666664</v>
+      </c>
+      <c r="AG5" s="5">
+        <v>-1.1654166666666583</v>
+      </c>
+      <c r="AH5" s="5">
+        <v>-2.065416666666664</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>2.8345833333333417</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>8.3345833333333417</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>2.8345833333333417</v>
+      </c>
+      <c r="AL5" s="5">
+        <v>7.1345833333333388</v>
+      </c>
+      <c r="AM5" s="5">
+        <v>5.434583333333336</v>
+      </c>
+      <c r="AN5" s="5">
+        <v>2.7345833333333331</v>
+      </c>
+      <c r="AO5" s="5">
+        <v>11.334583333333342</v>
+      </c>
+      <c r="AP5" s="5">
+        <v>15.434583333333336</v>
+      </c>
+      <c r="AQ5" s="5">
+        <v>19.434583333333336</v>
+      </c>
+      <c r="AR5" s="5">
+        <v>27.634583333333339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44">
+      <c r="A6" s="1">
+        <v>43612</v>
+      </c>
+      <c r="B6">
+        <v>-8.2104166666666814</v>
+      </c>
+      <c r="C6">
+        <v>-10.26541666666666</v>
+      </c>
+      <c r="D6">
+        <v>-10.320833333333326</v>
+      </c>
+      <c r="E6">
+        <v>-8.2875000000000085</v>
+      </c>
+      <c r="G6" s="1">
+        <v>43585</v>
+      </c>
+      <c r="H6">
+        <v>-7.5499999999999972</v>
+      </c>
+      <c r="I6">
+        <v>-4.9999999999997158E-2</v>
+      </c>
+      <c r="J6">
+        <v>3.6500000000000057</v>
+      </c>
+      <c r="K6">
+        <v>3.9500000000000028</v>
+      </c>
+      <c r="M6">
+        <v>26</v>
+      </c>
+      <c r="N6">
+        <v>-8.2104166666666671</v>
+      </c>
+      <c r="O6">
+        <v>-10.26541666666666</v>
+      </c>
+      <c r="P6">
+        <v>-10.32083333333334</v>
+      </c>
+      <c r="Q6">
+        <v>-8.2875000000000085</v>
+      </c>
+      <c r="T6" t="s">
+        <v>3</v>
+      </c>
+      <c r="U6" s="5">
+        <v>-32.520833333333343</v>
+      </c>
+      <c r="V6" s="5">
+        <v>-21.32083333333334</v>
+      </c>
+      <c r="W6" s="5">
+        <v>-15.32083333333334</v>
+      </c>
+      <c r="X6" s="5">
+        <v>-13.620833333333337</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>-10.32083333333334</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>4.17916666666666</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>-6.7208333333333456</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>-9.9208333333333343</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>2.0791666666666657</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>-7.1208333333333371</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>-2.7208333333333456</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>-2.1208333333333371</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>2.9791666666666572</v>
+      </c>
+      <c r="AH6" s="5">
+        <v>2.3791666666666629</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>-1.82083333333334</v>
+      </c>
+      <c r="AJ6" s="5">
+        <v>8.3791666666666629</v>
+      </c>
+      <c r="AK6" s="5">
+        <v>4.3791666666666629</v>
+      </c>
+      <c r="AL6" s="5">
+        <v>7.4791666666666572</v>
+      </c>
+      <c r="AM6" s="5">
+        <v>8.7791666666666544</v>
+      </c>
+      <c r="AN6" s="5">
+        <v>5.9791666666666572</v>
+      </c>
+      <c r="AO6" s="5">
+        <v>13.979166666666657</v>
+      </c>
+      <c r="AP6" s="5">
+        <v>15.17916666666666</v>
+      </c>
+      <c r="AQ6" s="5">
+        <v>16.479166666666657</v>
+      </c>
+      <c r="AR6" s="5">
+        <v>31.279166666666654</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44">
+      <c r="A7" s="1">
+        <v>43584</v>
+      </c>
+      <c r="B7">
+        <v>-6.4104166666666771</v>
+      </c>
+      <c r="C7">
+        <v>18.034583333333345</v>
+      </c>
+      <c r="D7">
+        <v>4.1791666666666742</v>
+      </c>
+      <c r="E7">
+        <v>-10.387500000000017</v>
+      </c>
+      <c r="G7" s="1">
+        <v>43600</v>
+      </c>
+      <c r="H7">
+        <v>-5.625</v>
+      </c>
+      <c r="I7">
+        <v>0.67499999999999716</v>
+      </c>
+      <c r="J7">
+        <v>3.2750000000000057</v>
+      </c>
+      <c r="K7">
+        <v>1.6749999999999972</v>
+      </c>
+      <c r="M7">
+        <v>-2</v>
+      </c>
+      <c r="N7">
+        <v>-6.4104166666666629</v>
+      </c>
+      <c r="O7">
+        <v>18.034583333333345</v>
+      </c>
+      <c r="P7">
+        <v>4.17916666666666</v>
+      </c>
+      <c r="Q7">
+        <v>-10.387500000000017</v>
+      </c>
+      <c r="T7" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="5">
+        <v>-34.687500000000014</v>
+      </c>
+      <c r="V7" s="5">
+        <v>-19.987500000000011</v>
+      </c>
+      <c r="W7" s="5">
+        <v>-15.487500000000011</v>
+      </c>
+      <c r="X7" s="5">
+        <v>-14.987500000000011</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>-8.2875000000000085</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>-10.387500000000017</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>-3.9875000000000114</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>-9.1875000000000142</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>-8.7500000000005684E-2</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>-5.1875000000000142</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>-0.58750000000000568</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>2.2124999999999915</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>3.3124999999999858</v>
+      </c>
+      <c r="AH7" s="5">
+        <v>2.7124999999999915</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>0.11249999999998295</v>
+      </c>
+      <c r="AJ7" s="5">
+        <v>9.4124999999999943</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>3.1124999999999829</v>
+      </c>
+      <c r="AL7" s="5">
+        <v>7.3124999999999858</v>
+      </c>
+      <c r="AM7" s="5">
+        <v>8.0124999999999886</v>
+      </c>
+      <c r="AN7" s="5">
+        <v>4.6124999999999829</v>
+      </c>
+      <c r="AO7" s="5">
+        <v>13.912499999999994</v>
+      </c>
+      <c r="AP7" s="5">
+        <v>17.212499999999991</v>
+      </c>
+      <c r="AQ7" s="5">
+        <v>19.412499999999994</v>
+      </c>
+      <c r="AR7" s="5">
+        <v>31.512499999999989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44">
+      <c r="A8" s="1">
+        <v>43572</v>
+      </c>
+      <c r="B8">
+        <v>-5.8604166666666799</v>
+      </c>
+      <c r="C8">
+        <v>-3.4954166666666566</v>
+      </c>
+      <c r="D8">
+        <v>-6.7208333333333314</v>
+      </c>
+      <c r="E8">
+        <v>-3.9875000000000114</v>
+      </c>
+      <c r="G8" s="1">
+        <v>43601</v>
+      </c>
+      <c r="H8">
+        <v>-1.0499999999999972</v>
+      </c>
+      <c r="I8">
+        <v>-1.25</v>
+      </c>
+      <c r="J8">
+        <v>0.84999999999999432</v>
+      </c>
+      <c r="K8">
+        <v>1.4500000000000028</v>
+      </c>
+      <c r="M8">
+        <v>-14</v>
+      </c>
+      <c r="N8">
+        <v>-5.8604166666666657</v>
+      </c>
+      <c r="O8">
+        <v>-3.4954166666666566</v>
+      </c>
+      <c r="P8">
+        <v>-6.7208333333333456</v>
+      </c>
+      <c r="Q8">
+        <v>-3.9875000000000114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44">
+      <c r="A9" s="1">
+        <v>43601</v>
+      </c>
+      <c r="B9">
+        <v>-5.2104166666666742</v>
+      </c>
+      <c r="C9">
+        <v>-8.6654166666666583</v>
+      </c>
+      <c r="D9">
+        <v>-9.9208333333333201</v>
+      </c>
+      <c r="E9">
+        <v>-9.1875000000000142</v>
+      </c>
+      <c r="G9" s="1">
+        <v>43602</v>
+      </c>
+      <c r="H9">
+        <v>-2.4249999999999972</v>
+      </c>
+      <c r="I9">
+        <v>1.0750000000000028</v>
+      </c>
+      <c r="J9">
+        <v>0.97499999999999432</v>
+      </c>
+      <c r="K9">
+        <v>0.375</v>
+      </c>
+      <c r="M9">
+        <v>15</v>
+      </c>
+      <c r="N9">
+        <v>-5.21041666666666</v>
+      </c>
+      <c r="O9">
+        <v>-8.6654166666666583</v>
+      </c>
+      <c r="P9">
+        <v>-9.9208333333333343</v>
+      </c>
+      <c r="Q9">
+        <v>-9.1875000000000142</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44">
+      <c r="A10" s="1">
+        <v>43613</v>
+      </c>
+      <c r="B10">
+        <v>-4.9104166666666771</v>
+      </c>
+      <c r="C10">
+        <v>-5.4654166666666555</v>
+      </c>
+      <c r="D10">
+        <v>2.0791666666666799</v>
+      </c>
+      <c r="E10">
+        <v>-8.7500000000005684E-2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>43603</v>
+      </c>
+      <c r="H10">
+        <v>-5.0750000000000028</v>
+      </c>
+      <c r="I10">
+        <v>-3.375</v>
+      </c>
+      <c r="J10">
+        <v>3.7249999999999943</v>
+      </c>
+      <c r="K10">
+        <v>4.7249999999999943</v>
+      </c>
+      <c r="M10">
+        <v>27</v>
+      </c>
+      <c r="N10">
+        <v>-4.9104166666666629</v>
+      </c>
+      <c r="O10">
+        <v>-5.4654166666666555</v>
+      </c>
+      <c r="P10">
+        <v>2.0791666666666657</v>
+      </c>
+      <c r="Q10">
+        <v>-8.7500000000005684E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44">
+      <c r="A11" s="1">
+        <v>43591</v>
+      </c>
+      <c r="B11">
+        <v>-3.8104166666666828</v>
+      </c>
+      <c r="C11">
+        <v>-5.1654166666666583</v>
+      </c>
+      <c r="D11">
+        <v>-7.1208333333333229</v>
+      </c>
+      <c r="E11">
+        <v>-5.1875000000000142</v>
+      </c>
+      <c r="G11" s="1">
+        <v>43605</v>
+      </c>
+      <c r="H11">
+        <v>-2.3999999999999986</v>
+      </c>
+      <c r="I11">
+        <v>-2.6000000000000014</v>
+      </c>
+      <c r="J11">
+        <v>2.5</v>
+      </c>
+      <c r="K11">
+        <v>2.5</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>-3.8104166666666686</v>
+      </c>
+      <c r="O11">
+        <v>-5.1654166666666583</v>
+      </c>
+      <c r="P11">
+        <v>-7.1208333333333371</v>
+      </c>
+      <c r="Q11">
+        <v>-5.1875000000000142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44">
+      <c r="A12" s="1">
+        <v>43611</v>
+      </c>
+      <c r="B12">
+        <v>-2.2104166666666742</v>
+      </c>
+      <c r="C12">
+        <v>-4.065416666666664</v>
+      </c>
+      <c r="D12">
+        <v>-2.7208333333333314</v>
+      </c>
+      <c r="E12">
+        <v>-0.58750000000000568</v>
+      </c>
+      <c r="G12" s="1">
+        <v>43584</v>
+      </c>
+      <c r="H12">
+        <v>-11.850000000000009</v>
+      </c>
+      <c r="I12">
+        <v>15.849999999999994</v>
+      </c>
+      <c r="J12">
+        <v>-9.9500000000000171</v>
+      </c>
+      <c r="K12">
+        <v>5.9499999999999886</v>
+      </c>
+      <c r="M12">
+        <v>25</v>
+      </c>
+      <c r="N12">
+        <v>-2.21041666666666</v>
+      </c>
+      <c r="O12">
+        <v>-4.065416666666664</v>
+      </c>
+      <c r="P12">
+        <v>-2.7208333333333456</v>
+      </c>
+      <c r="Q12">
+        <v>-0.58750000000000568</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44">
+      <c r="A13" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B13">
+        <v>-1.1104166666666799</v>
+      </c>
+      <c r="C13">
+        <v>-1.565416666666664</v>
+      </c>
+      <c r="D13">
+        <v>-2.1208333333333229</v>
+      </c>
+      <c r="E13">
+        <v>2.2124999999999915</v>
+      </c>
+      <c r="G13" s="1">
+        <v>43606</v>
+      </c>
+      <c r="H13">
+        <v>-3.5249999999999915</v>
+      </c>
+      <c r="I13">
+        <v>-1.6249999999999858</v>
+      </c>
+      <c r="J13">
+        <v>1.2750000000000057</v>
+      </c>
+      <c r="K13">
+        <v>3.8750000000000142</v>
+      </c>
+      <c r="M13">
+        <v>24</v>
+      </c>
+      <c r="N13">
+        <v>-1.1104166666666657</v>
+      </c>
+      <c r="O13">
+        <v>-1.565416666666664</v>
+      </c>
+      <c r="P13">
+        <v>-2.1208333333333371</v>
+      </c>
+      <c r="Q13">
+        <v>2.2124999999999915</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44">
+      <c r="A14" s="1">
+        <v>43603</v>
+      </c>
+      <c r="B14">
+        <v>0.38958333333332007</v>
+      </c>
+      <c r="C14">
+        <v>-1.1654166666666583</v>
+      </c>
+      <c r="D14">
+        <v>2.9791666666666714</v>
+      </c>
+      <c r="E14">
+        <v>3.3124999999999858</v>
+      </c>
+      <c r="G14" s="1">
+        <v>43607</v>
+      </c>
+      <c r="H14">
+        <v>-2.9500000000000028</v>
+      </c>
+      <c r="I14">
+        <v>-1.8500000000000014</v>
+      </c>
+      <c r="J14">
+        <v>1.6499999999999986</v>
+      </c>
+      <c r="K14">
+        <v>3.1499999999999986</v>
+      </c>
+      <c r="M14">
+        <v>17</v>
+      </c>
+      <c r="N14">
+        <v>0.38958333333333428</v>
+      </c>
+      <c r="O14">
+        <v>-1.1654166666666583</v>
+      </c>
+      <c r="P14">
+        <v>2.9791666666666572</v>
+      </c>
+      <c r="Q14">
+        <v>3.3124999999999858</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44">
+      <c r="A15" s="1">
+        <v>43608</v>
+      </c>
+      <c r="B15">
+        <v>0.58958333333332291</v>
+      </c>
+      <c r="C15">
+        <v>-2.065416666666664</v>
+      </c>
+      <c r="D15">
+        <v>2.3791666666666771</v>
+      </c>
+      <c r="E15">
+        <v>2.7124999999999915</v>
+      </c>
+      <c r="G15" s="1">
+        <v>43608</v>
+      </c>
+      <c r="H15">
+        <v>-4.3999999999999915</v>
+      </c>
+      <c r="I15">
+        <v>-3.7999999999999972</v>
+      </c>
+      <c r="J15">
+        <v>3.6000000000000085</v>
+      </c>
+      <c r="K15">
+        <v>4.6000000000000085</v>
+      </c>
+      <c r="M15">
+        <v>22</v>
+      </c>
+      <c r="N15">
+        <v>0.58958333333333712</v>
+      </c>
+      <c r="O15">
+        <v>-2.065416666666664</v>
+      </c>
+      <c r="P15">
+        <v>2.3791666666666629</v>
+      </c>
+      <c r="Q15">
+        <v>2.7124999999999915</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44">
+      <c r="A16" s="1">
+        <v>43602</v>
+      </c>
+      <c r="B16">
+        <v>2.5895833333333229</v>
+      </c>
+      <c r="C16">
+        <v>2.8345833333333417</v>
+      </c>
+      <c r="D16">
+        <v>-1.8208333333333258</v>
+      </c>
+      <c r="E16">
+        <v>0.11249999999998295</v>
+      </c>
+      <c r="G16" s="1">
+        <v>43609</v>
+      </c>
+      <c r="H16">
+        <v>-4.7999999999999972</v>
+      </c>
+      <c r="I16">
+        <v>-1.0999999999999943</v>
+      </c>
+      <c r="J16">
+        <v>3.3000000000000114</v>
+      </c>
+      <c r="K16">
+        <v>2.6000000000000085</v>
+      </c>
+      <c r="M16">
+        <v>16</v>
+      </c>
+      <c r="N16">
+        <v>2.5895833333333371</v>
+      </c>
+      <c r="O16">
+        <v>2.8345833333333417</v>
+      </c>
+      <c r="P16">
+        <v>-1.82083333333334</v>
+      </c>
+      <c r="Q16">
+        <v>0.11249999999998295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" s="1">
+        <v>43585</v>
+      </c>
+      <c r="B17">
+        <v>4.0895833333333229</v>
+      </c>
+      <c r="C17">
+        <v>8.3345833333333417</v>
+      </c>
+      <c r="D17">
+        <v>8.3791666666666771</v>
+      </c>
+      <c r="E17">
+        <v>9.4124999999999943</v>
+      </c>
+      <c r="G17" s="1">
+        <v>43610</v>
+      </c>
+      <c r="H17">
+        <v>-4.5499999999999972</v>
+      </c>
+      <c r="I17">
+        <v>-1.75</v>
+      </c>
+      <c r="J17">
+        <v>4.6500000000000057</v>
+      </c>
+      <c r="K17">
+        <v>1.6500000000000057</v>
+      </c>
+      <c r="M17">
+        <v>-1</v>
+      </c>
+      <c r="N17">
+        <v>4.0895833333333371</v>
+      </c>
+      <c r="O17">
+        <v>8.3345833333333417</v>
+      </c>
+      <c r="P17">
+        <v>8.3791666666666629</v>
+      </c>
+      <c r="Q17">
+        <v>9.4124999999999943</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" s="1">
+        <v>43606</v>
+      </c>
+      <c r="B18">
+        <v>4.1895833333333172</v>
+      </c>
+      <c r="C18">
+        <v>2.8345833333333417</v>
+      </c>
+      <c r="D18">
+        <v>4.3791666666666771</v>
+      </c>
+      <c r="E18">
+        <v>3.1124999999999829</v>
+      </c>
+      <c r="G18" s="1">
+        <v>43611</v>
+      </c>
+      <c r="H18">
+        <v>-3.8999999999999915</v>
+      </c>
+      <c r="I18">
+        <v>-2.5</v>
+      </c>
+      <c r="J18">
+        <v>3.6000000000000085</v>
+      </c>
+      <c r="K18">
+        <v>2.7999999999999972</v>
+      </c>
+      <c r="M18">
+        <v>20</v>
+      </c>
+      <c r="N18">
+        <v>4.1895833333333314</v>
+      </c>
+      <c r="O18">
+        <v>2.8345833333333417</v>
+      </c>
+      <c r="P18">
+        <v>4.3791666666666629</v>
+      </c>
+      <c r="Q18">
+        <v>3.1124999999999829</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" s="1">
+        <v>43578</v>
+      </c>
+      <c r="B19">
+        <v>5.0895833333333229</v>
+      </c>
+      <c r="C19">
+        <v>7.1345833333333388</v>
+      </c>
+      <c r="D19">
+        <v>7.4791666666666714</v>
+      </c>
+      <c r="E19">
+        <v>7.3124999999999858</v>
+      </c>
+      <c r="G19" s="1">
+        <v>43612</v>
+      </c>
+      <c r="H19">
+        <v>-3.0249999999999986</v>
+      </c>
+      <c r="I19">
+        <v>-1.8249999999999957</v>
+      </c>
+      <c r="J19">
+        <v>2.7750000000000057</v>
+      </c>
+      <c r="K19">
+        <v>2.0750000000000028</v>
+      </c>
+      <c r="M19">
+        <v>-8</v>
+      </c>
+      <c r="N19">
+        <v>5.0895833333333371</v>
+      </c>
+      <c r="O19">
+        <v>7.1345833333333388</v>
+      </c>
+      <c r="P19">
+        <v>7.4791666666666572</v>
+      </c>
+      <c r="Q19">
+        <v>7.3124999999999858</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" s="1">
+        <v>43595</v>
+      </c>
+      <c r="B20">
+        <v>6.7895833333333258</v>
+      </c>
+      <c r="C20">
+        <v>5.434583333333336</v>
+      </c>
+      <c r="D20">
+        <v>8.7791666666666686</v>
+      </c>
+      <c r="E20">
+        <v>8.0124999999999886</v>
+      </c>
+      <c r="G20" s="1">
+        <v>43613</v>
+      </c>
+      <c r="H20">
+        <v>-6.9000000000000057</v>
+      </c>
+      <c r="I20">
+        <v>-4.2000000000000028</v>
+      </c>
+      <c r="J20">
+        <v>3.7999999999999972</v>
+      </c>
+      <c r="K20">
+        <v>7.2999999999999972</v>
+      </c>
+      <c r="M20">
+        <v>9</v>
+      </c>
+      <c r="N20">
+        <v>6.78958333333334</v>
+      </c>
+      <c r="O20">
+        <v>5.434583333333336</v>
+      </c>
+      <c r="P20">
+        <v>8.7791666666666544</v>
+      </c>
+      <c r="Q20">
+        <v>8.0124999999999886</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" s="1">
+        <v>43593</v>
+      </c>
+      <c r="B21">
+        <v>8.1895833333333172</v>
+      </c>
+      <c r="C21">
+        <v>2.7345833333333331</v>
+      </c>
+      <c r="D21">
+        <v>5.9791666666666714</v>
+      </c>
+      <c r="E21">
+        <v>4.6124999999999829</v>
+      </c>
+      <c r="G21" s="1">
+        <v>43616</v>
+      </c>
+      <c r="H21">
+        <v>-4.3250000000000028</v>
+      </c>
+      <c r="I21">
+        <v>2.875</v>
+      </c>
+      <c r="J21">
+        <v>-0.625</v>
+      </c>
+      <c r="K21">
+        <v>2.0750000000000028</v>
+      </c>
+      <c r="M21">
+        <v>7</v>
+      </c>
+      <c r="N21">
+        <v>8.1895833333333314</v>
+      </c>
+      <c r="O21">
+        <v>2.7345833333333331</v>
+      </c>
+      <c r="P21">
+        <v>5.9791666666666572</v>
+      </c>
+      <c r="Q21">
+        <v>4.6124999999999829</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" s="1">
+        <v>43580</v>
+      </c>
+      <c r="B22">
+        <v>13.289583333333326</v>
+      </c>
+      <c r="C22">
+        <v>11.334583333333342</v>
+      </c>
+      <c r="D22">
+        <v>13.979166666666671</v>
+      </c>
+      <c r="E22">
+        <v>13.912499999999994</v>
+      </c>
+      <c r="G22" s="1">
+        <v>43629</v>
+      </c>
+      <c r="H22">
+        <v>1.4000000000000057</v>
+      </c>
+      <c r="I22">
+        <v>-1.2999999999999972</v>
+      </c>
+      <c r="J22">
+        <v>-1.7999999999999972</v>
+      </c>
+      <c r="K22">
+        <v>1.7000000000000028</v>
+      </c>
+      <c r="M22">
+        <v>-6</v>
+      </c>
+      <c r="N22">
+        <v>13.28958333333334</v>
+      </c>
+      <c r="O22">
+        <v>11.334583333333342</v>
+      </c>
+      <c r="P22">
+        <v>13.979166666666657</v>
+      </c>
+      <c r="Q22">
+        <v>13.912499999999994</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" s="1">
+        <v>43609</v>
+      </c>
+      <c r="B23">
+        <v>14.989583333333314</v>
+      </c>
+      <c r="C23">
+        <v>15.434583333333336</v>
+      </c>
+      <c r="D23">
+        <v>15.179166666666674</v>
+      </c>
+      <c r="E23">
+        <v>17.212499999999991</v>
+      </c>
+      <c r="G23" s="1">
+        <v>43580</v>
+      </c>
+      <c r="H23">
+        <v>-3.9250000000000114</v>
+      </c>
+      <c r="I23">
+        <v>-2.6250000000000142</v>
+      </c>
+      <c r="J23">
+        <v>2.5749999999999886</v>
+      </c>
+      <c r="K23">
+        <v>3.9749999999999801</v>
+      </c>
+      <c r="M23">
+        <v>23</v>
+      </c>
+      <c r="N23">
+        <v>14.989583333333329</v>
+      </c>
+      <c r="O23">
+        <v>15.434583333333336</v>
+      </c>
+      <c r="P23">
+        <v>15.17916666666666</v>
+      </c>
+      <c r="Q23">
+        <v>17.212499999999991</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="1">
+        <v>43600</v>
+      </c>
+      <c r="B24">
+        <v>16.38958333333332</v>
+      </c>
+      <c r="C24">
+        <v>19.434583333333336</v>
+      </c>
+      <c r="D24">
+        <v>16.479166666666671</v>
+      </c>
+      <c r="E24">
+        <v>19.412499999999994</v>
+      </c>
+      <c r="G24" s="1">
+        <v>43578</v>
+      </c>
+      <c r="H24">
+        <v>-5.75</v>
+      </c>
+      <c r="I24">
+        <v>-0.45000000000000284</v>
+      </c>
+      <c r="J24">
+        <v>2.3499999999999943</v>
+      </c>
+      <c r="K24">
+        <v>3.8499999999999943</v>
+      </c>
+      <c r="M24">
+        <v>14</v>
+      </c>
+      <c r="N24">
+        <v>16.389583333333334</v>
+      </c>
+      <c r="O24">
+        <v>19.434583333333336</v>
+      </c>
+      <c r="P24">
+        <v>16.479166666666657</v>
+      </c>
+      <c r="Q24">
+        <v>19.412499999999994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" s="1">
+        <v>43587</v>
+      </c>
+      <c r="B25">
+        <v>32.789583333333326</v>
+      </c>
+      <c r="C25">
+        <v>27.634583333333339</v>
+      </c>
+      <c r="D25">
+        <v>31.279166666666669</v>
+      </c>
+      <c r="E25">
+        <v>31.512499999999989</v>
+      </c>
+      <c r="G25" s="1">
+        <v>43572</v>
+      </c>
+      <c r="H25">
+        <v>-4.9300000000000068</v>
+      </c>
+      <c r="I25">
+        <v>0.68999999999999773</v>
+      </c>
+      <c r="J25">
+        <v>2.8199999999999932</v>
+      </c>
+      <c r="K25">
+        <v>1.4199999999999875</v>
+      </c>
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>32.78958333333334</v>
+      </c>
+      <c r="O25">
+        <v>27.634583333333339</v>
+      </c>
+      <c r="P25">
+        <v>31.279166666666654</v>
+      </c>
+      <c r="Q25">
+        <v>31.512499999999989</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M2:Q25">
+    <sortCondition ref="N2:N25"/>
+    <sortCondition ref="O2:O25"/>
+    <sortCondition ref="P2:P25"/>
+    <sortCondition ref="Q2:Q25"/>
+  </sortState>
+  <conditionalFormatting sqref="B2:E25">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -5638,828 +7314,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="1">
-        <v>43629</v>
-      </c>
-      <c r="B2">
-        <v>-25.61041666666668</v>
-      </c>
-      <c r="C2">
-        <v>-31.565416666666664</v>
-      </c>
-      <c r="D2">
-        <v>-32.520833333333329</v>
-      </c>
-      <c r="E2">
-        <v>-34.687500000000014</v>
-      </c>
-      <c r="G2" s="1">
-        <v>43587</v>
-      </c>
-      <c r="H2">
-        <v>-2.0999999999999943</v>
-      </c>
-      <c r="I2">
-        <v>-4</v>
-      </c>
-      <c r="J2">
-        <v>2.5</v>
-      </c>
-      <c r="K2">
-        <v>3.5999999999999943</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="1">
-        <v>43605</v>
-      </c>
-      <c r="B3">
-        <v>-19.010416666666679</v>
-      </c>
-      <c r="C3">
-        <v>-22.465416666666663</v>
-      </c>
-      <c r="D3">
-        <v>-21.320833333333326</v>
-      </c>
-      <c r="E3">
-        <v>-19.987500000000011</v>
-      </c>
-      <c r="G3" s="1">
-        <v>43591</v>
-      </c>
-      <c r="H3">
-        <v>-2.5750000000000028</v>
-      </c>
-      <c r="I3">
-        <v>-0.67499999999999716</v>
-      </c>
-      <c r="J3">
-        <v>1.9249999999999972</v>
-      </c>
-      <c r="K3">
-        <v>1.3250000000000028</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="1">
-        <v>43607</v>
-      </c>
-      <c r="B4">
-        <v>-14.210416666666681</v>
-      </c>
-      <c r="C4">
-        <v>-16.365416666666661</v>
-      </c>
-      <c r="D4">
-        <v>-15.320833333333326</v>
-      </c>
-      <c r="E4">
-        <v>-15.487500000000011</v>
-      </c>
-      <c r="G4" s="1">
-        <v>43593</v>
-      </c>
-      <c r="H4">
-        <v>-1.2749999999999915</v>
-      </c>
-      <c r="I4">
-        <v>-3.4749999999999943</v>
-      </c>
-      <c r="J4">
-        <v>1.0250000000000057</v>
-      </c>
-      <c r="K4">
-        <v>3.7250000000000085</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="1">
-        <v>43616</v>
-      </c>
-      <c r="B5">
-        <v>-12.810416666666683</v>
-      </c>
-      <c r="C5">
-        <v>-8.8654166666666612</v>
-      </c>
-      <c r="D5">
-        <v>-13.620833333333323</v>
-      </c>
-      <c r="E5">
-        <v>-14.987500000000011</v>
-      </c>
-      <c r="G5" s="1">
-        <v>43595</v>
-      </c>
-      <c r="H5">
-        <v>-4.5499999999999829</v>
-      </c>
-      <c r="I5">
-        <v>-2.6499999999999915</v>
-      </c>
-      <c r="J5">
-        <v>2.5500000000000114</v>
-      </c>
-      <c r="K5">
-        <v>4.6500000000000057</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="1">
-        <v>43612</v>
-      </c>
-      <c r="B6">
-        <v>-8.2104166666666814</v>
-      </c>
-      <c r="C6">
-        <v>-10.26541666666666</v>
-      </c>
-      <c r="D6">
-        <v>-10.320833333333326</v>
-      </c>
-      <c r="E6">
-        <v>-8.2875000000000085</v>
-      </c>
-      <c r="G6" s="1">
-        <v>43585</v>
-      </c>
-      <c r="H6">
-        <v>-7.5499999999999972</v>
-      </c>
-      <c r="I6">
-        <v>-4.9999999999997158E-2</v>
-      </c>
-      <c r="J6">
-        <v>3.6500000000000057</v>
-      </c>
-      <c r="K6">
-        <v>3.9500000000000028</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="1">
-        <v>43584</v>
-      </c>
-      <c r="B7">
-        <v>-6.4104166666666771</v>
-      </c>
-      <c r="C7">
-        <v>18.034583333333345</v>
-      </c>
-      <c r="D7">
-        <v>4.1791666666666742</v>
-      </c>
-      <c r="E7">
-        <v>-10.387500000000017</v>
-      </c>
-      <c r="G7" s="1">
-        <v>43600</v>
-      </c>
-      <c r="H7">
-        <v>-5.625</v>
-      </c>
-      <c r="I7">
-        <v>0.67499999999999716</v>
-      </c>
-      <c r="J7">
-        <v>3.2750000000000057</v>
-      </c>
-      <c r="K7">
-        <v>1.6749999999999972</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="1">
-        <v>43572</v>
-      </c>
-      <c r="B8">
-        <v>-5.8604166666666799</v>
-      </c>
-      <c r="C8">
-        <v>-3.4954166666666566</v>
-      </c>
-      <c r="D8">
-        <v>-6.7208333333333314</v>
-      </c>
-      <c r="E8">
-        <v>-3.9875000000000114</v>
-      </c>
-      <c r="G8" s="1">
-        <v>43601</v>
-      </c>
-      <c r="H8">
-        <v>-1.0499999999999972</v>
-      </c>
-      <c r="I8">
-        <v>-1.25</v>
-      </c>
-      <c r="J8">
-        <v>0.84999999999999432</v>
-      </c>
-      <c r="K8">
-        <v>1.4500000000000028</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="1">
-        <v>43601</v>
-      </c>
-      <c r="B9">
-        <v>-5.2104166666666742</v>
-      </c>
-      <c r="C9">
-        <v>-8.6654166666666583</v>
-      </c>
-      <c r="D9">
-        <v>-9.9208333333333201</v>
-      </c>
-      <c r="E9">
-        <v>-9.1875000000000142</v>
-      </c>
-      <c r="G9" s="1">
-        <v>43602</v>
-      </c>
-      <c r="H9">
-        <v>-2.4249999999999972</v>
-      </c>
-      <c r="I9">
-        <v>1.0750000000000028</v>
-      </c>
-      <c r="J9">
-        <v>0.97499999999999432</v>
-      </c>
-      <c r="K9">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="1">
-        <v>43613</v>
-      </c>
-      <c r="B10">
-        <v>-4.9104166666666771</v>
-      </c>
-      <c r="C10">
-        <v>-5.4654166666666555</v>
-      </c>
-      <c r="D10">
-        <v>2.0791666666666799</v>
-      </c>
-      <c r="E10">
-        <v>-8.7500000000005684E-2</v>
-      </c>
-      <c r="G10" s="1">
-        <v>43603</v>
-      </c>
-      <c r="H10">
-        <v>-5.0750000000000028</v>
-      </c>
-      <c r="I10">
-        <v>-3.375</v>
-      </c>
-      <c r="J10">
-        <v>3.7249999999999943</v>
-      </c>
-      <c r="K10">
-        <v>4.7249999999999943</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="1">
-        <v>43591</v>
-      </c>
-      <c r="B11">
-        <v>-3.8104166666666828</v>
-      </c>
-      <c r="C11">
-        <v>-5.1654166666666583</v>
-      </c>
-      <c r="D11">
-        <v>-7.1208333333333229</v>
-      </c>
-      <c r="E11">
-        <v>-5.1875000000000142</v>
-      </c>
-      <c r="G11" s="1">
-        <v>43605</v>
-      </c>
-      <c r="H11">
-        <v>-2.3999999999999986</v>
-      </c>
-      <c r="I11">
-        <v>-2.6000000000000014</v>
-      </c>
-      <c r="J11">
-        <v>2.5</v>
-      </c>
-      <c r="K11">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="1">
-        <v>43611</v>
-      </c>
-      <c r="B12">
-        <v>-2.2104166666666742</v>
-      </c>
-      <c r="C12">
-        <v>-4.065416666666664</v>
-      </c>
-      <c r="D12">
-        <v>-2.7208333333333314</v>
-      </c>
-      <c r="E12">
-        <v>-0.58750000000000568</v>
-      </c>
-      <c r="G12" s="1">
-        <v>43584</v>
-      </c>
-      <c r="H12">
-        <v>-11.850000000000009</v>
-      </c>
-      <c r="I12">
-        <v>15.849999999999994</v>
-      </c>
-      <c r="J12">
-        <v>-9.9500000000000171</v>
-      </c>
-      <c r="K12">
-        <v>5.9499999999999886</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1">
-        <v>43610</v>
-      </c>
-      <c r="B13">
-        <v>-1.1104166666666799</v>
-      </c>
-      <c r="C13">
-        <v>-1.565416666666664</v>
-      </c>
-      <c r="D13">
-        <v>-2.1208333333333229</v>
-      </c>
-      <c r="E13">
-        <v>2.2124999999999915</v>
-      </c>
-      <c r="G13" s="1">
-        <v>43606</v>
-      </c>
-      <c r="H13">
-        <v>-3.5249999999999915</v>
-      </c>
-      <c r="I13">
-        <v>-1.6249999999999858</v>
-      </c>
-      <c r="J13">
-        <v>1.2750000000000057</v>
-      </c>
-      <c r="K13">
-        <v>3.8750000000000142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1">
-        <v>43603</v>
-      </c>
-      <c r="B14">
-        <v>0.38958333333332007</v>
-      </c>
-      <c r="C14">
-        <v>-1.1654166666666583</v>
-      </c>
-      <c r="D14">
-        <v>2.9791666666666714</v>
-      </c>
-      <c r="E14">
-        <v>3.3124999999999858</v>
-      </c>
-      <c r="G14" s="1">
-        <v>43607</v>
-      </c>
-      <c r="H14">
-        <v>-2.9500000000000028</v>
-      </c>
-      <c r="I14">
-        <v>-1.8500000000000014</v>
-      </c>
-      <c r="J14">
-        <v>1.6499999999999986</v>
-      </c>
-      <c r="K14">
-        <v>3.1499999999999986</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="1">
-        <v>43608</v>
-      </c>
-      <c r="B15">
-        <v>0.58958333333332291</v>
-      </c>
-      <c r="C15">
-        <v>-2.065416666666664</v>
-      </c>
-      <c r="D15">
-        <v>2.3791666666666771</v>
-      </c>
-      <c r="E15">
-        <v>2.7124999999999915</v>
-      </c>
-      <c r="G15" s="1">
-        <v>43608</v>
-      </c>
-      <c r="H15">
-        <v>-4.3999999999999915</v>
-      </c>
-      <c r="I15">
-        <v>-3.7999999999999972</v>
-      </c>
-      <c r="J15">
-        <v>3.6000000000000085</v>
-      </c>
-      <c r="K15">
-        <v>4.6000000000000085</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="1">
-        <v>43602</v>
-      </c>
-      <c r="B16">
-        <v>2.5895833333333229</v>
-      </c>
-      <c r="C16">
-        <v>2.8345833333333417</v>
-      </c>
-      <c r="D16">
-        <v>-1.8208333333333258</v>
-      </c>
-      <c r="E16">
-        <v>0.11249999999998295</v>
-      </c>
-      <c r="G16" s="1">
-        <v>43609</v>
-      </c>
-      <c r="H16">
-        <v>-4.7999999999999972</v>
-      </c>
-      <c r="I16">
-        <v>-1.0999999999999943</v>
-      </c>
-      <c r="J16">
-        <v>3.3000000000000114</v>
-      </c>
-      <c r="K16">
-        <v>2.6000000000000085</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="1">
-        <v>43585</v>
-      </c>
-      <c r="B17">
-        <v>4.0895833333333229</v>
-      </c>
-      <c r="C17">
-        <v>8.3345833333333417</v>
-      </c>
-      <c r="D17">
-        <v>8.3791666666666771</v>
-      </c>
-      <c r="E17">
-        <v>9.4124999999999943</v>
-      </c>
-      <c r="G17" s="1">
-        <v>43610</v>
-      </c>
-      <c r="H17">
-        <v>-4.5499999999999972</v>
-      </c>
-      <c r="I17">
-        <v>-1.75</v>
-      </c>
-      <c r="J17">
-        <v>4.6500000000000057</v>
-      </c>
-      <c r="K17">
-        <v>1.6500000000000057</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="1">
-        <v>43606</v>
-      </c>
-      <c r="B18">
-        <v>4.1895833333333172</v>
-      </c>
-      <c r="C18">
-        <v>2.8345833333333417</v>
-      </c>
-      <c r="D18">
-        <v>4.3791666666666771</v>
-      </c>
-      <c r="E18">
-        <v>3.1124999999999829</v>
-      </c>
-      <c r="G18" s="1">
-        <v>43611</v>
-      </c>
-      <c r="H18">
-        <v>-3.8999999999999915</v>
-      </c>
-      <c r="I18">
-        <v>-2.5</v>
-      </c>
-      <c r="J18">
-        <v>3.6000000000000085</v>
-      </c>
-      <c r="K18">
-        <v>2.7999999999999972</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="1">
-        <v>43578</v>
-      </c>
-      <c r="B19">
-        <v>5.0895833333333229</v>
-      </c>
-      <c r="C19">
-        <v>7.1345833333333388</v>
-      </c>
-      <c r="D19">
-        <v>7.4791666666666714</v>
-      </c>
-      <c r="E19">
-        <v>7.3124999999999858</v>
-      </c>
-      <c r="G19" s="1">
-        <v>43612</v>
-      </c>
-      <c r="H19">
-        <v>-3.0249999999999986</v>
-      </c>
-      <c r="I19">
-        <v>-1.8249999999999957</v>
-      </c>
-      <c r="J19">
-        <v>2.7750000000000057</v>
-      </c>
-      <c r="K19">
-        <v>2.0750000000000028</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="1">
-        <v>43595</v>
-      </c>
-      <c r="B20">
-        <v>6.7895833333333258</v>
-      </c>
-      <c r="C20">
-        <v>5.434583333333336</v>
-      </c>
-      <c r="D20">
-        <v>8.7791666666666686</v>
-      </c>
-      <c r="E20">
-        <v>8.0124999999999886</v>
-      </c>
-      <c r="G20" s="1">
-        <v>43613</v>
-      </c>
-      <c r="H20">
-        <v>-6.9000000000000057</v>
-      </c>
-      <c r="I20">
-        <v>-4.2000000000000028</v>
-      </c>
-      <c r="J20">
-        <v>3.7999999999999972</v>
-      </c>
-      <c r="K20">
-        <v>7.2999999999999972</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="1">
-        <v>43593</v>
-      </c>
-      <c r="B21">
-        <v>8.1895833333333172</v>
-      </c>
-      <c r="C21">
-        <v>2.7345833333333331</v>
-      </c>
-      <c r="D21">
-        <v>5.9791666666666714</v>
-      </c>
-      <c r="E21">
-        <v>4.6124999999999829</v>
-      </c>
-      <c r="G21" s="1">
-        <v>43616</v>
-      </c>
-      <c r="H21">
-        <v>-4.3250000000000028</v>
-      </c>
-      <c r="I21">
-        <v>2.875</v>
-      </c>
-      <c r="J21">
-        <v>-0.625</v>
-      </c>
-      <c r="K21">
-        <v>2.0750000000000028</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="1">
-        <v>43580</v>
-      </c>
-      <c r="B22">
-        <v>13.289583333333326</v>
-      </c>
-      <c r="C22">
-        <v>11.334583333333342</v>
-      </c>
-      <c r="D22">
-        <v>13.979166666666671</v>
-      </c>
-      <c r="E22">
-        <v>13.912499999999994</v>
-      </c>
-      <c r="G22" s="1">
-        <v>43629</v>
-      </c>
-      <c r="H22">
-        <v>1.4000000000000057</v>
-      </c>
-      <c r="I22">
-        <v>-1.2999999999999972</v>
-      </c>
-      <c r="J22">
-        <v>-1.7999999999999972</v>
-      </c>
-      <c r="K22">
-        <v>1.7000000000000028</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="1">
-        <v>43609</v>
-      </c>
-      <c r="B23">
-        <v>14.989583333333314</v>
-      </c>
-      <c r="C23">
-        <v>15.434583333333336</v>
-      </c>
-      <c r="D23">
-        <v>15.179166666666674</v>
-      </c>
-      <c r="E23">
-        <v>17.212499999999991</v>
-      </c>
-      <c r="G23" s="1">
-        <v>43580</v>
-      </c>
-      <c r="H23">
-        <v>-3.9250000000000114</v>
-      </c>
-      <c r="I23">
-        <v>-2.6250000000000142</v>
-      </c>
-      <c r="J23">
-        <v>2.5749999999999886</v>
-      </c>
-      <c r="K23">
-        <v>3.9749999999999801</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="1">
-        <v>43600</v>
-      </c>
-      <c r="B24">
-        <v>16.38958333333332</v>
-      </c>
-      <c r="C24">
-        <v>19.434583333333336</v>
-      </c>
-      <c r="D24">
-        <v>16.479166666666671</v>
-      </c>
-      <c r="E24">
-        <v>19.412499999999994</v>
-      </c>
-      <c r="G24" s="1">
-        <v>43578</v>
-      </c>
-      <c r="H24">
-        <v>-5.75</v>
-      </c>
-      <c r="I24">
-        <v>-0.45000000000000284</v>
-      </c>
-      <c r="J24">
-        <v>2.3499999999999943</v>
-      </c>
-      <c r="K24">
-        <v>3.8499999999999943</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="1">
-        <v>43587</v>
-      </c>
-      <c r="B25">
-        <v>32.789583333333326</v>
-      </c>
-      <c r="C25">
-        <v>27.634583333333339</v>
-      </c>
-      <c r="D25">
-        <v>31.279166666666669</v>
-      </c>
-      <c r="E25">
-        <v>31.512499999999989</v>
-      </c>
-      <c r="G25" s="1">
-        <v>43572</v>
-      </c>
-      <c r="H25">
-        <v>-4.9300000000000068</v>
-      </c>
-      <c r="I25">
-        <v>0.68999999999999773</v>
-      </c>
-      <c r="J25">
-        <v>2.8199999999999932</v>
-      </c>
-      <c r="K25">
-        <v>1.4199999999999875</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
-    <sortCondition ref="B2:B25"/>
-    <sortCondition ref="C2:C25"/>
-    <sortCondition ref="D2:D25"/>
-    <sortCondition ref="E2:E25"/>
-  </sortState>
-  <conditionalFormatting sqref="B2:E25">
+  <conditionalFormatting sqref="H2:K25">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:Q25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -6471,7 +7338,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:K25">
+  <conditionalFormatting sqref="U4:AR7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>